<commit_message>
added .gitignore and .gitattributes, made minor changes to coworker notebooks
</commit_message>
<xml_diff>
--- a/wti模型3.0/data_input_auto/PADD3炼厂压裂裂解.xlsx
+++ b/wti模型3.0/data_input_auto/PADD3炼厂压裂裂解.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3613"/>
+  <dimension ref="A1:D3615"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -47007,11 +47007,39 @@
       <c r="A3613" s="2" t="n">
         <v>45954</v>
       </c>
-      <c r="B3613" t="inlineStr"/>
+      <c r="B3613" t="n">
+        <v>22.93</v>
+      </c>
       <c r="C3613" t="n">
-        <v>16.98</v>
-      </c>
-      <c r="D3613" t="inlineStr"/>
+        <v>17.09</v>
+      </c>
+      <c r="D3613" t="n">
+        <v>38.43</v>
+      </c>
+    </row>
+    <row r="3614">
+      <c r="A3614" s="2" t="n">
+        <v>45957</v>
+      </c>
+      <c r="B3614" t="n">
+        <v>22.11</v>
+      </c>
+      <c r="C3614" t="n">
+        <v>17.21</v>
+      </c>
+      <c r="D3614" t="n">
+        <v>39.91</v>
+      </c>
+    </row>
+    <row r="3615">
+      <c r="A3615" s="2" t="n">
+        <v>45958</v>
+      </c>
+      <c r="B3615" t="inlineStr"/>
+      <c r="C3615" t="n">
+        <v>17.98</v>
+      </c>
+      <c r="D3615" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>